<commit_message>
[dengchangyou] handle parse float issue
</commit_message>
<xml_diff>
--- a/test/sample_etl_wps.syntax.xlsx
+++ b/test/sample_etl_wps.syntax.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/changyoudeng/project/easy_sql/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302C6ECC-FDFD-124C-9A97-36CA323F1D5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD22C4BA-3A49-E344-BFA3-89D3C37181B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="28000" windowHeight="17240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Suit 1" sheetId="2" r:id="rId1"/>
@@ -127,7 +127,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -157,6 +157,11 @@
       <sz val="9"/>
       <name val="Times New Roman"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -184,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -198,6 +203,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,7 +425,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -454,7 +460,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1">
-      <c r="B4">
+      <c r="B4" s="9">
         <v>1</v>
       </c>
       <c r="C4">

</xml_diff>

<commit_message>
fix: fix wps template issue
</commit_message>
<xml_diff>
--- a/test/sample_etl_wps.syntax.xlsx
+++ b/test/sample_etl_wps.syntax.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/changyoudeng/project/easy_sql/test/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD22C4BA-3A49-E344-BFA3-89D3C37181B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28000" windowHeight="17240"/>
   </bookViews>
   <sheets>
     <sheet name="Suit 1" sheetId="2" r:id="rId1"/>
@@ -20,18 +14,19 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>gmliao</author>
   </authors>
   <commentList>
-    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="B14" authorId="0">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="Times New Roman"/>
+            <charset val="0"/>
           </rPr>
           <t>Comment for each row of input data is required. This is designed to improve test readability.</t>
         </r>
@@ -42,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29">
   <si>
     <t>CASE</t>
   </si>
@@ -111,6 +106,9 @@
     <t>Some sample data for testing</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>OUTPUT</t>
   </si>
   <si>
@@ -120,14 +118,26 @@
     <t>2021-01-01</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>null</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="24">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -153,17 +163,158 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="9"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,8 +327,194 @@
         <bgColor rgb="FF666666"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -185,11 +522,253 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -200,22 +779,65 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1"/>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -413,28 +1035,27 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="5"/>
   <cols>
-    <col min="2" max="2" width="26.33203125" customWidth="1"/>
-    <col min="3" max="3" width="43.1640625" customWidth="1"/>
+    <col min="2" max="2" width="26.2857142857143" customWidth="1"/>
+    <col min="3" max="3" width="43.1517857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -442,7 +1063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+    <row r="3" customHeight="1" spans="1:5">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -459,8 +1080,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
-      <c r="B4" s="9">
+    <row r="4" customHeight="1" spans="2:5">
+      <c r="B4">
         <v>1</v>
       </c>
       <c r="C4">
@@ -473,7 +1094,7 @@
         <v>44197</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1">
+    <row r="6" customHeight="1" spans="1:3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -484,7 +1105,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1">
+    <row r="8" customHeight="1" spans="1:2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -492,7 +1113,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="28">
+    <row r="10" ht="24" spans="1:3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -503,7 +1124,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="28">
+    <row r="11" ht="24" spans="2:3">
       <c r="B11" t="s">
         <v>14</v>
       </c>
@@ -511,7 +1132,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="13">
+    <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -531,15 +1152,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="17">
+    <row r="14" ht="15" spans="2:6">
       <c r="B14" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
       </c>
-      <c r="D14" s="7">
-        <v>1</v>
+      <c r="D14" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="E14" s="6">
         <v>44197</v>
@@ -548,12 +1169,12 @@
         <v>44197</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="13">
+    <row r="16" ht="12" spans="1:5">
       <c r="A16" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>17</v>
@@ -565,39 +1186,40 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="3:5" ht="13">
+    <row r="17" ht="12" spans="3:5">
       <c r="C17" s="1">
         <v>1</v>
       </c>
-      <c r="D17" s="7">
-        <v>1</v>
+      <c r="D17" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="18" spans="3:5" ht="15.75" customHeight="1">
+    <row r="18" customHeight="1" spans="3:5">
       <c r="C18" s="1">
         <v>1</v>
       </c>
-      <c r="D18" s="7">
-        <v>2</v>
+      <c r="D18" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="E18" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="19" spans="3:5" ht="15.75" customHeight="1">
+    <row r="19" customHeight="1" spans="3:5">
       <c r="C19" s="1">
         <v>1</v>
       </c>
-      <c r="D19" s="7">
-        <v>3</v>
+      <c r="D19" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="E19" s="6"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>